<commit_message>
updated sentence evaluation scripts and readme files
</commit_message>
<xml_diff>
--- a/experiments/20110202_manual_sentence_selection/Sentence_evaluation.xlsx
+++ b/experiments/20110202_manual_sentence_selection/Sentence_evaluation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>Bahn</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -87,6 +87,24 @@
   <si>
     <t>Ben</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bahn</t>
+  </si>
+  <si>
+    <t>ben</t>
+  </si>
+  <si>
+    <t>auto-first</t>
+  </si>
+  <si>
+    <t>auto-recent</t>
+  </si>
+  <si>
+    <t>auto-self</t>
+  </si>
+  <si>
+    <t>auto-self2</t>
   </si>
 </sst>
 </file>
@@ -461,10 +479,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -731,8 +749,313 @@
         <v>0.48</v>
       </c>
     </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>0.5</v>
+      </c>
+      <c r="D13">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="E13">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="F13">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="G13">
+        <v>0.75</v>
+      </c>
+      <c r="H13">
+        <v>0.79500000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D14">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="E14">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="F14">
+        <v>0.34</v>
+      </c>
+      <c r="G14">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="H14">
+        <v>0.36199999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D15">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="E15">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="F15">
+        <v>0.32</v>
+      </c>
+      <c r="G15">
+        <v>0.41</v>
+      </c>
+      <c r="H15">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="C16">
+        <f>AVERAGE(C14:C15)</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D16">
+        <f>AVERAGE(D14:D15)</f>
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="F16">
+        <f>AVERAGE(F14:F15)</f>
+        <v>0.33</v>
+      </c>
+      <c r="G16">
+        <f>AVERAGE(G14:G15)</f>
+        <v>0.39800000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="D18">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="E18">
+        <v>0.39</v>
+      </c>
+      <c r="F18">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="G18">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="H18">
+        <v>0.58099999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="D19">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="E19">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="F19">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="G19">
+        <v>0.59</v>
+      </c>
+      <c r="H19">
+        <v>0.52300000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="C20">
+        <f>AVERAGE(C18:C19)</f>
+        <v>0.30649999999999999</v>
+      </c>
+      <c r="D20">
+        <f>AVERAGE(D18:D19)</f>
+        <v>0.437</v>
+      </c>
+      <c r="F20">
+        <f>AVERAGE(F18:F19)</f>
+        <v>0.51</v>
+      </c>
+      <c r="G20">
+        <f>AVERAGE(G18:G19)</f>
+        <v>0.60199999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="D22">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="E22">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="F22">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="G22">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="H22">
+        <v>0.47099999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23">
+        <v>0.317</v>
+      </c>
+      <c r="D23">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="E23">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="F23">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="G23">
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="H23">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="C24">
+        <f>AVERAGE(C22:C23)</f>
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="D24">
+        <f>AVERAGE(D22:D23)</f>
+        <v>0.36249999999999999</v>
+      </c>
+      <c r="F24">
+        <f>AVERAGE(F22:F23)</f>
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="G24">
+        <f>AVERAGE(G22:G23)</f>
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="D26">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="E26">
+        <v>0.39</v>
+      </c>
+      <c r="F26">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="G26">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="H26">
+        <v>0.55900000000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="D27">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="E27">
+        <v>0.376</v>
+      </c>
+      <c r="F27">
+        <v>0.51</v>
+      </c>
+      <c r="G27">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="H27">
+        <v>0.56799999999999995</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="C28">
+        <f>AVERAGE(C26:C27)</f>
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="D28">
+        <f>AVERAGE(D26:D27)</f>
+        <v>0.46450000000000002</v>
+      </c>
+      <c r="F28">
+        <f>AVERAGE(F26:F27)</f>
+        <v>0.52049999999999996</v>
+      </c>
+      <c r="G28">
+        <f>AVERAGE(G26:G27)</f>
+        <v>0.61599999999999999</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>